<commit_message>
almost ready for gpt
</commit_message>
<xml_diff>
--- a/cropped_and_labeled_figs.xlsx
+++ b/cropped_and_labeled_figs.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -510,7 +510,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Process Diagram</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I2" t="b">
@@ -547,7 +547,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Conceptual Diagram</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I3" t="b">
@@ -584,7 +584,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Scatter Plot</t>
+          <t>scatter plot</t>
         </is>
       </c>
       <c r="I4" t="b">
@@ -621,7 +621,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Conceptual Diagram</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I5" t="b">
@@ -658,7 +658,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Conceptual Diagram</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I6" t="b">
@@ -695,7 +695,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I7" t="b">
@@ -732,7 +732,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Conceptual Diagram</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I8" t="b">
@@ -769,7 +769,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Conceptual Diagram</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I9" t="b">
@@ -806,7 +806,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I10" t="b">
@@ -843,7 +843,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Process Diagram</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I11" t="b">
@@ -880,7 +880,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I12" t="b">
@@ -917,7 +917,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I13" t="b">
@@ -954,7 +954,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I14" t="b">
@@ -991,7 +991,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I15" t="b">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I16" t="b">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I17" t="b">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I18" t="b">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I19" t="b">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Data structure</t>
+          <t>data structure</t>
         </is>
       </c>
       <c r="I20" t="b">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I21" t="b">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I22" t="b">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I23" t="b">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I24" t="b">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I25" t="b">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I26" t="b">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I27" t="b">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I28" t="b">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Data structure</t>
+          <t>data structure</t>
         </is>
       </c>
       <c r="I29" t="b">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I30" t="b">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I31" t="b">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Cycle</t>
+          <t>cycle</t>
         </is>
       </c>
       <c r="I32" t="b">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Drawing</t>
+          <t>drawing</t>
         </is>
       </c>
       <c r="I33" t="b">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I34" t="b">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I35" t="b">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Data structure</t>
+          <t>data structure</t>
         </is>
       </c>
       <c r="I36" t="b">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I37" t="b">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I38" t="b">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2x2 Matrix</t>
+          <t>2x2 matrix</t>
         </is>
       </c>
       <c r="I39" t="b">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I40" t="b">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Organizational Chart</t>
+          <t>organizational chart</t>
         </is>
       </c>
       <c r="I41" t="b">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2x2 Matrix</t>
+          <t>2x2 matrix</t>
         </is>
       </c>
       <c r="I42" t="b">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Process Diagram</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I43" t="b">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Data structure</t>
+          <t>data structure</t>
         </is>
       </c>
       <c r="I44" t="b">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cycle</t>
+          <t>cycle</t>
         </is>
       </c>
       <c r="I45" t="b">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I46" t="b">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I47" t="b">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Photo</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I48" t="b">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Process Diagram</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I49" t="b">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cycle</t>
+          <t>cycle</t>
         </is>
       </c>
       <c r="I50" t="b">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I51" t="b">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I52" t="b">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I53" t="b">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Drawing</t>
+          <t>drawing</t>
         </is>
       </c>
       <c r="I54" t="b">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Drawing</t>
+          <t>drawing</t>
         </is>
       </c>
       <c r="I55" t="b">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I56" t="b">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I57" t="b">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I58" t="b">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Data display</t>
+          <t>data display</t>
         </is>
       </c>
       <c r="I59" t="b">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I60" t="b">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Process Diagram</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I61" t="b">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I62" t="b">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I63" t="b">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>None Selected</t>
+          <t>none selected</t>
         </is>
       </c>
       <c r="I64" t="b">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Data structure</t>
+          <t>data structure</t>
         </is>
       </c>
       <c r="I65" t="b">

</xml_diff>

<commit_message>
openai classification script complete
</commit_message>
<xml_diff>
--- a/cropped_and_labeled_figs.xlsx
+++ b/cropped_and_labeled_figs.xlsx
@@ -695,7 +695,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>2x2 matrix</t>
         </is>
       </c>
       <c r="I7" t="b">
@@ -806,7 +806,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I10" t="b">
@@ -880,7 +880,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I12" t="b">
@@ -917,7 +917,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I13" t="b">
@@ -954,7 +954,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I14" t="b">
@@ -991,7 +991,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I15" t="b">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I16" t="b">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I17" t="b">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I18" t="b">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I19" t="b">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I22" t="b">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>cycle</t>
         </is>
       </c>
       <c r="I24" t="b">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>cycle</t>
         </is>
       </c>
       <c r="I25" t="b">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I26" t="b">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>mixed statistical plot (more than 1 statistical plot type)</t>
         </is>
       </c>
       <c r="I30" t="b">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I31" t="b">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I34" t="b">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>cycle</t>
         </is>
       </c>
       <c r="I35" t="b">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I37" t="b">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I38" t="b">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I51" t="b">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I52" t="b">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I53" t="b">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>process diagram</t>
         </is>
       </c>
       <c r="I56" t="b">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I57" t="b">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I58" t="b">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>photo</t>
         </is>
       </c>
       <c r="I60" t="b">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I62" t="b">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I63" t="b">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>none selected</t>
+          <t>conceptual diagram</t>
         </is>
       </c>
       <c r="I64" t="b">

</xml_diff>